<commit_message>
create project detail for user non-administration
</commit_message>
<xml_diff>
--- a/public/timeline_template.xlsx
+++ b/public/timeline_template.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\vue\vue-collectiva\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059CDCB9-581B-46D5-ADC7-35F96DF01491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F663B20-BC8E-465C-8337-875C5A1B97E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="1770" windowWidth="9060" windowHeight="7590" xr2:uid="{65A70969-1D21-4F52-A81E-EA74BE4AE9AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{65A70969-1D21-4F52-A81E-EA74BE4AE9AA}"/>
   </bookViews>
   <sheets>
     <sheet name="contoh timeline" sheetId="1" r:id="rId1"/>
+    <sheet name="List Icon" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>date</t>
   </si>
@@ -969,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD6DCA6-7F0C-4DB0-A49C-049B1958FB66}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1109,4 +1110,34 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD99092-AED9-436E-8CD4-E3CA37D05975}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>